<commit_message>
aktualizace vzoru, aby datumy byly v jednom mesici
</commit_message>
<xml_diff>
--- a/data/CMPA_template_cz.xlsx
+++ b/data/CMPA_template_cz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horkyt\Desktop\sablony pro novy internetovy model\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\TomasT\TomasT\fnx_for_tasks\494\predelane sablony pro CMPA release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EC84B6-F8E2-4D4C-856C-092CB69207E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA7F796-2E10-419C-B03B-745FA1B2B307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="4005" windowWidth="28800" windowHeight="15045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spoty" sheetId="2" r:id="rId1"/>
@@ -1199,7 +1199,7 @@
     <cellStyle name="8" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="9" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Název 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Normální 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
     <cellStyle name="Normální 3" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="Normální 4" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
@@ -1647,7 +1647,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="6">
-        <v>45097</v>
+        <v>45127</v>
       </c>
       <c r="H3" s="3">
         <v>0.81254629629629627</v>
@@ -1668,7 +1668,7 @@
         <v>30</v>
       </c>
       <c r="F4" s="6">
-        <v>45098</v>
+        <v>45128</v>
       </c>
       <c r="H4" s="3">
         <v>0.8125</v>
@@ -1689,7 +1689,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="6">
-        <v>45099</v>
+        <v>45129</v>
       </c>
       <c r="H5" s="3">
         <v>0.8125</v>
@@ -1713,7 +1713,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="6">
-        <v>45097</v>
+        <v>45127</v>
       </c>
       <c r="H6" s="3">
         <v>0.33320601851851855</v>
@@ -1737,7 +1737,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="6">
-        <v>45098</v>
+        <v>45128</v>
       </c>
       <c r="H7" s="3">
         <v>0.33320601851851855</v>
@@ -1761,7 +1761,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="6">
-        <v>45100</v>
+        <v>45130</v>
       </c>
       <c r="H8" s="3">
         <v>0.85416666666666696</v>
@@ -1782,7 +1782,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="6">
-        <v>45096</v>
+        <v>45126</v>
       </c>
       <c r="J9">
         <v>150000</v>
@@ -1799,7 +1799,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="6">
-        <v>45097</v>
+        <v>45127</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>53</v>
       </c>
       <c r="F11" s="6">
-        <v>45099</v>
+        <v>45129</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1827,10 +1827,10 @@
         <v>28</v>
       </c>
       <c r="F12" s="6">
-        <v>45089</v>
+        <v>45119</v>
       </c>
       <c r="G12" s="6">
-        <v>45097</v>
+        <v>45127</v>
       </c>
       <c r="K12">
         <v>20000</v>
@@ -1865,10 +1865,10 @@
         <v>55</v>
       </c>
       <c r="F13" s="6">
-        <v>45049</v>
+        <v>45110</v>
       </c>
       <c r="G13" s="6">
-        <v>45049</v>
+        <v>45110</v>
       </c>
       <c r="K13">
         <v>15000</v>
@@ -1897,10 +1897,10 @@
         <v>71</v>
       </c>
       <c r="F14" s="6">
-        <v>45097</v>
+        <v>45127</v>
       </c>
       <c r="G14" s="6">
-        <v>45099</v>
+        <v>45129</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>

</xml_diff>